<commit_message>
aggiornamento BR e gestione override
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="57">
   <si>
     <t>Action</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>INDICATOR_33</t>
+  </si>
+  <si>
+    <t>INDICATOR_12_OVER</t>
   </si>
 </sst>
 </file>
@@ -873,10 +876,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1570,6 +1573,23 @@
         <v>14</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1617,6 +1637,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1730,7 +1756,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1739,13 +1765,22 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1761,25 +1796,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiunta indicatori italia modulo CR SISTEMA
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="68">
   <si>
     <t>Action</t>
   </si>
@@ -274,6 +274,39 @@
   </si>
   <si>
     <t>INDICATOR_12_OVER</t>
+  </si>
+  <si>
+    <t>INDICATOR_50</t>
+  </si>
+  <si>
+    <t>INDICATOR_51</t>
+  </si>
+  <si>
+    <t>INDICATOR_52</t>
+  </si>
+  <si>
+    <t>INDICATOR_53</t>
+  </si>
+  <si>
+    <t>INDICATOR_54</t>
+  </si>
+  <si>
+    <t>INDICATOR_200</t>
+  </si>
+  <si>
+    <t>INDICATOR_201</t>
+  </si>
+  <si>
+    <t>INDICATOR_202</t>
+  </si>
+  <si>
+    <t>INDICATOR_203</t>
+  </si>
+  <si>
+    <t>INDICATOR_204</t>
+  </si>
+  <si>
+    <t>INDICATOR_205</t>
   </si>
 </sst>
 </file>
@@ -876,10 +909,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1593,6 +1626,193 @@
         <v>14</v>
       </c>
     </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1605,7 +1825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1637,9 +1857,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1757,25 +1980,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1797,9 +2010,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
caricamento indicatori CR alzo zero e xra corporate
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="53625" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="74">
   <si>
     <t>Action</t>
   </si>
@@ -307,6 +307,24 @@
   </si>
   <si>
     <t>INDICATOR_205</t>
+  </si>
+  <si>
+    <t>INDICATOR_55</t>
+  </si>
+  <si>
+    <t>INDICATOR_56</t>
+  </si>
+  <si>
+    <t>INDICATOR_57</t>
+  </si>
+  <si>
+    <t>INDICATOR_58</t>
+  </si>
+  <si>
+    <t>INDICATOR_60</t>
+  </si>
+  <si>
+    <t>INDICATOR_61</t>
   </si>
 </sst>
 </file>
@@ -909,10 +927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="C44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56:F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1813,6 +1831,108 @@
         <v>14</v>
       </c>
     </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1825,7 +1945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1857,12 +1977,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1980,15 +2097,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2010,16 +2137,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
AGGIORNAMENTO MODULI CR SISTEMA, ALZO ZER E XRA
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="105">
   <si>
     <t>Action</t>
   </si>
@@ -325,6 +325,99 @@
   </si>
   <si>
     <t>INDICATOR_61</t>
+  </si>
+  <si>
+    <t>INDICATOR_206</t>
+  </si>
+  <si>
+    <t>INDICATOR_207</t>
+  </si>
+  <si>
+    <t>INDICATOR_208</t>
+  </si>
+  <si>
+    <t>INDICATOR_209</t>
+  </si>
+  <si>
+    <t>INDICATOR_210</t>
+  </si>
+  <si>
+    <t>INDICATOR_211</t>
+  </si>
+  <si>
+    <t>INDICATOR_212</t>
+  </si>
+  <si>
+    <t>INDICATOR_213</t>
+  </si>
+  <si>
+    <t>INDICATOR_214</t>
+  </si>
+  <si>
+    <t>INDICATOR_215</t>
+  </si>
+  <si>
+    <t>INDICATOR_216</t>
+  </si>
+  <si>
+    <t>INDICATOR_217</t>
+  </si>
+  <si>
+    <t>INDICATOR_218</t>
+  </si>
+  <si>
+    <t>INDICATOR_219</t>
+  </si>
+  <si>
+    <t>INDICATOR_220</t>
+  </si>
+  <si>
+    <t>INDICATOR_221</t>
+  </si>
+  <si>
+    <t>INDICATOR_222</t>
+  </si>
+  <si>
+    <t>INDICATOR_223</t>
+  </si>
+  <si>
+    <t>INDICATOR_224</t>
+  </si>
+  <si>
+    <t>INDICATOR_225</t>
+  </si>
+  <si>
+    <t>INDICATOR_226</t>
+  </si>
+  <si>
+    <t>INDICATOR_227</t>
+  </si>
+  <si>
+    <t>INDICATOR_228</t>
+  </si>
+  <si>
+    <t>INDICATOR_229</t>
+  </si>
+  <si>
+    <t>INDICATOR_230</t>
+  </si>
+  <si>
+    <t>INDICATOR_231</t>
+  </si>
+  <si>
+    <t>INDICATOR_232</t>
+  </si>
+  <si>
+    <t>INDICATOR_233</t>
+  </si>
+  <si>
+    <t>INDICATOR_234</t>
+  </si>
+  <si>
+    <t>INDICATOR_235</t>
+  </si>
+  <si>
+    <t>INDICATOR_236</t>
   </si>
 </sst>
 </file>
@@ -927,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56:F58"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59:F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1930,6 +2023,533 @@
         <v>14</v>
       </c>
       <c r="F58" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1977,12 +2597,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -2096,6 +2710,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2106,21 +2726,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2136,6 +2741,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
aggiornamento indicatore 59 e 54
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="106">
   <si>
     <t>Action</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>INDICATOR_236</t>
+  </si>
+  <si>
+    <t>INDICATOR_59</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G89"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59:F89"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89:F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2550,6 +2553,23 @@
         <v>14</v>
       </c>
       <c r="F89" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2597,6 +2617,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -2710,33 +2745,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2757,9 +2769,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggionramento ind fase1 e aggiunta ind fase2 - corporate
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="115">
   <si>
     <t>Action</t>
   </si>
@@ -421,6 +421,33 @@
   </si>
   <si>
     <t>INDICATOR_59</t>
+  </si>
+  <si>
+    <t>INDICATOR_62</t>
+  </si>
+  <si>
+    <t>INDICATOR_63</t>
+  </si>
+  <si>
+    <t>INDICATOR_64</t>
+  </si>
+  <si>
+    <t>INDICATOR_65</t>
+  </si>
+  <si>
+    <t>INDICATOR_66</t>
+  </si>
+  <si>
+    <t>INDICATOR_67</t>
+  </si>
+  <si>
+    <t>INDICATOR_68</t>
+  </si>
+  <si>
+    <t>INDICATOR_69</t>
+  </si>
+  <si>
+    <t>INDICATOR_70</t>
   </si>
 </sst>
 </file>
@@ -1023,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G90"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90:F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2570,6 +2597,159 @@
         <v>14</v>
       </c>
       <c r="F90" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2617,12 +2797,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2740,15 +2917,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2770,16 +2957,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiunta moduli indicatori fase 3
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="164">
   <si>
     <t>Action</t>
   </si>
@@ -448,6 +448,153 @@
   </si>
   <si>
     <t>INDICATOR_70</t>
+  </si>
+  <si>
+    <t>INDICATOR_71</t>
+  </si>
+  <si>
+    <t>INDICATOR_72</t>
+  </si>
+  <si>
+    <t>INDICATOR_73</t>
+  </si>
+  <si>
+    <t>INDICATOR_74</t>
+  </si>
+  <si>
+    <t>INDICATOR_75</t>
+  </si>
+  <si>
+    <t>INDICATOR_76</t>
+  </si>
+  <si>
+    <t>INDICATOR_77</t>
+  </si>
+  <si>
+    <t>INDICATOR_78</t>
+  </si>
+  <si>
+    <t>INDICATOR_79</t>
+  </si>
+  <si>
+    <t>INDICATOR_80</t>
+  </si>
+  <si>
+    <t>INDICATOR_237</t>
+  </si>
+  <si>
+    <t>INDICATOR_238</t>
+  </si>
+  <si>
+    <t>INDICATOR_239</t>
+  </si>
+  <si>
+    <t>INDICATOR_240</t>
+  </si>
+  <si>
+    <t>INDICATOR_241</t>
+  </si>
+  <si>
+    <t>INDICATOR_242</t>
+  </si>
+  <si>
+    <t>INDICATOR_243</t>
+  </si>
+  <si>
+    <t>INDICATOR_244</t>
+  </si>
+  <si>
+    <t>INDICATOR_245</t>
+  </si>
+  <si>
+    <t>INDICATOR_246</t>
+  </si>
+  <si>
+    <t>INDICATOR_247</t>
+  </si>
+  <si>
+    <t>INDICATOR_248</t>
+  </si>
+  <si>
+    <t>INDICATOR_249</t>
+  </si>
+  <si>
+    <t>INDICATOR_250</t>
+  </si>
+  <si>
+    <t>INDICATOR_251</t>
+  </si>
+  <si>
+    <t>INDICATOR_252</t>
+  </si>
+  <si>
+    <t>INDICATOR_253</t>
+  </si>
+  <si>
+    <t>INDICATOR_254</t>
+  </si>
+  <si>
+    <t>INDICATOR_255</t>
+  </si>
+  <si>
+    <t>INDICATOR_256</t>
+  </si>
+  <si>
+    <t>INDICATOR_257</t>
+  </si>
+  <si>
+    <t>INDICATOR_258</t>
+  </si>
+  <si>
+    <t>INDICATOR_259</t>
+  </si>
+  <si>
+    <t>INDICATOR_260</t>
+  </si>
+  <si>
+    <t>INDICATOR_261</t>
+  </si>
+  <si>
+    <t>INDICATOR_262</t>
+  </si>
+  <si>
+    <t>INDICATOR_263</t>
+  </si>
+  <si>
+    <t>INDICATOR_264</t>
+  </si>
+  <si>
+    <t>INDICATOR_265</t>
+  </si>
+  <si>
+    <t>INDICATOR_266</t>
+  </si>
+  <si>
+    <t>INDICATOR_267</t>
+  </si>
+  <si>
+    <t>INDICATOR_268</t>
+  </si>
+  <si>
+    <t>INDICATOR_269</t>
+  </si>
+  <si>
+    <t>INDICATOR_270</t>
+  </si>
+  <si>
+    <t>INDICATOR_271</t>
+  </si>
+  <si>
+    <t>INDICATOR_272</t>
+  </si>
+  <si>
+    <t>INDICATOR_273</t>
+  </si>
+  <si>
+    <t>INDICATOR_274</t>
+  </si>
+  <si>
+    <t>INDICATOR_275</t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90:F99"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2750,6 +2897,839 @@
         <v>14</v>
       </c>
       <c r="F99" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F143" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F144" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F146" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F147" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F148" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2797,12 +3777,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -2916,16 +3905,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2940,7 +3928,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2954,12 +3942,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiornamento indicatori high priority e forme indeterminate CR - XRA
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="175">
   <si>
     <t>Action</t>
   </si>
@@ -622,6 +622,12 @@
   </si>
   <si>
     <t>INDICATOR_32</t>
+  </si>
+  <si>
+    <t>INDICATOR_34</t>
+  </si>
+  <si>
+    <t>INDICATOR_35</t>
   </si>
 </sst>
 </file>
@@ -1224,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G157"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1880,8 +1886,8 @@
       <c r="B38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>33</v>
+      <c r="C38" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>14</v>
@@ -1897,8 +1903,8 @@
       <c r="B39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>46</v>
+      <c r="C39" s="5" t="s">
+        <v>173</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>14</v>
@@ -1914,8 +1920,8 @@
       <c r="B40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>45</v>
+      <c r="C40" s="5" t="s">
+        <v>174</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>14</v>
@@ -1931,8 +1937,8 @@
       <c r="B41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>47</v>
+      <c r="C41" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>14</v>
@@ -1949,7 +1955,7 @@
         <v>16</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>14</v>
@@ -1966,7 +1972,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>14</v>
@@ -1983,7 +1989,7 @@
         <v>16</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>14</v>
@@ -2000,7 +2006,7 @@
         <v>16</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>14</v>
@@ -2017,7 +2023,7 @@
         <v>16</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>14</v>
@@ -2034,7 +2040,7 @@
         <v>16</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>14</v>
@@ -2051,7 +2057,7 @@
         <v>16</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>14</v>
@@ -2068,7 +2074,7 @@
         <v>16</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>14</v>
@@ -2085,7 +2091,7 @@
         <v>16</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>14</v>
@@ -2102,7 +2108,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>14</v>
@@ -2119,7 +2125,7 @@
         <v>16</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>14</v>
@@ -2136,7 +2142,7 @@
         <v>16</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>14</v>
@@ -2153,7 +2159,7 @@
         <v>16</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>14</v>
@@ -2170,7 +2176,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>14</v>
@@ -2187,7 +2193,7 @@
         <v>16</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>14</v>
@@ -2204,7 +2210,7 @@
         <v>16</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>14</v>
@@ -2221,7 +2227,7 @@
         <v>16</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>14</v>
@@ -2238,7 +2244,7 @@
         <v>16</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>14</v>
@@ -2255,7 +2261,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>14</v>
@@ -2272,7 +2278,7 @@
         <v>16</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>14</v>
@@ -2289,7 +2295,7 @@
         <v>16</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>14</v>
@@ -2306,7 +2312,7 @@
         <v>16</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>14</v>
@@ -2323,7 +2329,7 @@
         <v>16</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>14</v>
@@ -2340,7 +2346,7 @@
         <v>16</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>14</v>
@@ -2357,7 +2363,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>14</v>
@@ -2374,7 +2380,7 @@
         <v>16</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>14</v>
@@ -2391,7 +2397,7 @@
         <v>16</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>14</v>
@@ -2408,7 +2414,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>14</v>
@@ -2425,7 +2431,7 @@
         <v>16</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>14</v>
@@ -2442,7 +2448,7 @@
         <v>16</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>14</v>
@@ -2459,7 +2465,7 @@
         <v>16</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>14</v>
@@ -2476,7 +2482,7 @@
         <v>16</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>14</v>
@@ -2493,7 +2499,7 @@
         <v>16</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>14</v>
@@ -2510,7 +2516,7 @@
         <v>16</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>14</v>
@@ -2527,7 +2533,7 @@
         <v>16</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>14</v>
@@ -2544,7 +2550,7 @@
         <v>16</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>14</v>
@@ -2561,7 +2567,7 @@
         <v>16</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>14</v>
@@ -2578,7 +2584,7 @@
         <v>16</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>14</v>
@@ -2595,7 +2601,7 @@
         <v>16</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>14</v>
@@ -2612,7 +2618,7 @@
         <v>16</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>14</v>
@@ -2629,7 +2635,7 @@
         <v>16</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>62</v>
+        <v>123</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>14</v>
@@ -2646,7 +2652,7 @@
         <v>16</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>63</v>
+        <v>124</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>14</v>
@@ -2663,7 +2669,7 @@
         <v>16</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>14</v>
@@ -2680,7 +2686,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>14</v>
@@ -2697,7 +2703,7 @@
         <v>16</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>14</v>
@@ -2714,7 +2720,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>14</v>
@@ -2731,7 +2737,7 @@
         <v>16</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>14</v>
@@ -2748,7 +2754,7 @@
         <v>16</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>14</v>
@@ -2765,7 +2771,7 @@
         <v>16</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>14</v>
@@ -2782,7 +2788,7 @@
         <v>16</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>14</v>
@@ -2799,7 +2805,7 @@
         <v>16</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>14</v>
@@ -2816,7 +2822,7 @@
         <v>16</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>14</v>
@@ -2833,7 +2839,7 @@
         <v>16</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>14</v>
@@ -2850,7 +2856,7 @@
         <v>16</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>14</v>
@@ -2867,7 +2873,7 @@
         <v>16</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>14</v>
@@ -2884,7 +2890,7 @@
         <v>16</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>14</v>
@@ -2901,7 +2907,7 @@
         <v>16</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>14</v>
@@ -2918,7 +2924,7 @@
         <v>16</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>14</v>
@@ -2935,7 +2941,7 @@
         <v>16</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>14</v>
@@ -2952,7 +2958,7 @@
         <v>16</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>14</v>
@@ -2969,7 +2975,7 @@
         <v>16</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>14</v>
@@ -2986,7 +2992,7 @@
         <v>16</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>14</v>
@@ -3003,7 +3009,7 @@
         <v>16</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>14</v>
@@ -3020,7 +3026,7 @@
         <v>16</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>14</v>
@@ -3037,7 +3043,7 @@
         <v>16</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>14</v>
@@ -3054,7 +3060,7 @@
         <v>16</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>14</v>
@@ -3071,7 +3077,7 @@
         <v>16</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>14</v>
@@ -3088,7 +3094,7 @@
         <v>16</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>14</v>
@@ -3105,7 +3111,7 @@
         <v>16</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>14</v>
@@ -3122,7 +3128,7 @@
         <v>16</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>14</v>
@@ -3139,7 +3145,7 @@
         <v>16</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>14</v>
@@ -3156,7 +3162,7 @@
         <v>16</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>14</v>
@@ -3173,7 +3179,7 @@
         <v>16</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>14</v>
@@ -3190,7 +3196,7 @@
         <v>16</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>14</v>
@@ -3207,7 +3213,7 @@
         <v>16</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>14</v>
@@ -3224,7 +3230,7 @@
         <v>16</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>14</v>
@@ -3241,7 +3247,7 @@
         <v>16</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>14</v>
@@ -3258,7 +3264,7 @@
         <v>16</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>14</v>
@@ -3275,7 +3281,7 @@
         <v>16</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>14</v>
@@ -3292,7 +3298,7 @@
         <v>16</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>14</v>
@@ -3309,7 +3315,7 @@
         <v>16</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>14</v>
@@ -3326,7 +3332,7 @@
         <v>16</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>14</v>
@@ -3343,7 +3349,7 @@
         <v>16</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>14</v>
@@ -3360,7 +3366,7 @@
         <v>16</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>14</v>
@@ -3377,7 +3383,7 @@
         <v>16</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>14</v>
@@ -3394,7 +3400,7 @@
         <v>16</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>14</v>
@@ -3411,7 +3417,7 @@
         <v>16</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>14</v>
@@ -3428,7 +3434,7 @@
         <v>16</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>14</v>
@@ -3445,7 +3451,7 @@
         <v>16</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>14</v>
@@ -3462,7 +3468,7 @@
         <v>16</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>14</v>
@@ -3479,7 +3485,7 @@
         <v>16</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>14</v>
@@ -3496,7 +3502,7 @@
         <v>16</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>14</v>
@@ -3513,7 +3519,7 @@
         <v>16</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>14</v>
@@ -3530,7 +3536,7 @@
         <v>16</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>14</v>
@@ -3547,7 +3553,7 @@
         <v>16</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>14</v>
@@ -3564,7 +3570,7 @@
         <v>16</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>14</v>
@@ -3581,7 +3587,7 @@
         <v>16</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>14</v>
@@ -3598,7 +3604,7 @@
         <v>16</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>14</v>
@@ -3615,7 +3621,7 @@
         <v>16</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>14</v>
@@ -3632,7 +3638,7 @@
         <v>16</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>14</v>
@@ -3649,7 +3655,7 @@
         <v>16</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>14</v>
@@ -3666,7 +3672,7 @@
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>14</v>
@@ -3683,7 +3689,7 @@
         <v>16</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>14</v>
@@ -3700,7 +3706,7 @@
         <v>16</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>14</v>
@@ -3717,7 +3723,7 @@
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>14</v>
@@ -3734,7 +3740,7 @@
         <v>16</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>14</v>
@@ -3751,7 +3757,7 @@
         <v>16</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>14</v>
@@ -3768,7 +3774,7 @@
         <v>16</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>14</v>
@@ -3785,7 +3791,7 @@
         <v>16</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>14</v>
@@ -3802,7 +3808,7 @@
         <v>16</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>14</v>
@@ -3819,7 +3825,7 @@
         <v>16</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>14</v>
@@ -3836,7 +3842,7 @@
         <v>16</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>14</v>
@@ -3853,7 +3859,7 @@
         <v>16</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>14</v>
@@ -3870,7 +3876,7 @@
         <v>16</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>14</v>
@@ -3887,7 +3893,7 @@
         <v>16</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>14</v>
@@ -3904,12 +3910,46 @@
         <v>16</v>
       </c>
       <c r="C157" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E157" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F157" s="1" t="s">
+      <c r="E159" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F159" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3957,6 +3997,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -4070,15 +4119,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -4086,6 +4126,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4097,14 +4145,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
aggiornamento indicatori cast e modifiche 80,81,82,83
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="178">
   <si>
     <t>Action</t>
   </si>
@@ -628,6 +628,15 @@
   </si>
   <si>
     <t>INDICATOR_35</t>
+  </si>
+  <si>
+    <t>INDICATOR_81</t>
+  </si>
+  <si>
+    <t>INDICATOR_82</t>
+  </si>
+  <si>
+    <t>INDICATOR_83</t>
   </si>
 </sst>
 </file>
@@ -1230,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:F40"/>
+    <sheetView tabSelected="1" topLeftCell="C72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83:F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2669,7 +2678,7 @@
         <v>16</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>62</v>
+        <v>175</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>14</v>
@@ -2686,7 +2695,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>63</v>
+        <v>176</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>14</v>
@@ -2703,7 +2712,7 @@
         <v>16</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>14</v>
@@ -2720,7 +2729,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>14</v>
@@ -2737,7 +2746,7 @@
         <v>16</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>14</v>
@@ -2754,7 +2763,7 @@
         <v>16</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>14</v>
@@ -2771,7 +2780,7 @@
         <v>16</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>14</v>
@@ -2788,7 +2797,7 @@
         <v>16</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>14</v>
@@ -2805,7 +2814,7 @@
         <v>16</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>14</v>
@@ -2822,7 +2831,7 @@
         <v>16</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>14</v>
@@ -2839,7 +2848,7 @@
         <v>16</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>14</v>
@@ -2856,7 +2865,7 @@
         <v>16</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>14</v>
@@ -2873,7 +2882,7 @@
         <v>16</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>14</v>
@@ -2890,7 +2899,7 @@
         <v>16</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>14</v>
@@ -2907,7 +2916,7 @@
         <v>16</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>14</v>
@@ -2924,7 +2933,7 @@
         <v>16</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>14</v>
@@ -2941,7 +2950,7 @@
         <v>16</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>14</v>
@@ -2958,7 +2967,7 @@
         <v>16</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>14</v>
@@ -2975,7 +2984,7 @@
         <v>16</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>14</v>
@@ -2992,7 +3001,7 @@
         <v>16</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>14</v>
@@ -3009,7 +3018,7 @@
         <v>16</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>14</v>
@@ -3026,7 +3035,7 @@
         <v>16</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>14</v>
@@ -3043,7 +3052,7 @@
         <v>16</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>14</v>
@@ -3060,7 +3069,7 @@
         <v>16</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>14</v>
@@ -3077,7 +3086,7 @@
         <v>16</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>14</v>
@@ -3094,7 +3103,7 @@
         <v>16</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>14</v>
@@ -3111,7 +3120,7 @@
         <v>16</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>14</v>
@@ -3128,7 +3137,7 @@
         <v>16</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>14</v>
@@ -3145,7 +3154,7 @@
         <v>16</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>14</v>
@@ -3162,7 +3171,7 @@
         <v>16</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>14</v>
@@ -3179,7 +3188,7 @@
         <v>16</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>14</v>
@@ -3196,7 +3205,7 @@
         <v>16</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>14</v>
@@ -3213,7 +3222,7 @@
         <v>16</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>14</v>
@@ -3230,7 +3239,7 @@
         <v>16</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>14</v>
@@ -3247,7 +3256,7 @@
         <v>16</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>14</v>
@@ -3264,7 +3273,7 @@
         <v>16</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>14</v>
@@ -3281,7 +3290,7 @@
         <v>16</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>14</v>
@@ -3298,7 +3307,7 @@
         <v>16</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>14</v>
@@ -3315,7 +3324,7 @@
         <v>16</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>14</v>
@@ -3332,7 +3341,7 @@
         <v>16</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>14</v>
@@ -3349,7 +3358,7 @@
         <v>16</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>14</v>
@@ -3366,7 +3375,7 @@
         <v>16</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>14</v>
@@ -3383,7 +3392,7 @@
         <v>16</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>14</v>
@@ -3400,7 +3409,7 @@
         <v>16</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>14</v>
@@ -3417,7 +3426,7 @@
         <v>16</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>14</v>
@@ -3434,7 +3443,7 @@
         <v>16</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>14</v>
@@ -3451,7 +3460,7 @@
         <v>16</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>14</v>
@@ -3468,7 +3477,7 @@
         <v>16</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>14</v>
@@ -3485,7 +3494,7 @@
         <v>16</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>14</v>
@@ -3502,7 +3511,7 @@
         <v>16</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>14</v>
@@ -3519,7 +3528,7 @@
         <v>16</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>14</v>
@@ -3536,7 +3545,7 @@
         <v>16</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>14</v>
@@ -3553,7 +3562,7 @@
         <v>16</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>14</v>
@@ -3570,7 +3579,7 @@
         <v>16</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>14</v>
@@ -3587,7 +3596,7 @@
         <v>16</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>14</v>
@@ -3604,7 +3613,7 @@
         <v>16</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>14</v>
@@ -3621,7 +3630,7 @@
         <v>16</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>14</v>
@@ -3638,7 +3647,7 @@
         <v>16</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>14</v>
@@ -3655,7 +3664,7 @@
         <v>16</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>14</v>
@@ -3672,7 +3681,7 @@
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>14</v>
@@ -3689,7 +3698,7 @@
         <v>16</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>14</v>
@@ -3706,7 +3715,7 @@
         <v>16</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>14</v>
@@ -3723,7 +3732,7 @@
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>14</v>
@@ -3740,7 +3749,7 @@
         <v>16</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>14</v>
@@ -3757,7 +3766,7 @@
         <v>16</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>14</v>
@@ -3774,7 +3783,7 @@
         <v>16</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>14</v>
@@ -3791,7 +3800,7 @@
         <v>16</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>14</v>
@@ -3808,7 +3817,7 @@
         <v>16</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>14</v>
@@ -3825,7 +3834,7 @@
         <v>16</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>14</v>
@@ -3842,7 +3851,7 @@
         <v>16</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>14</v>
@@ -3859,7 +3868,7 @@
         <v>16</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>14</v>
@@ -3876,7 +3885,7 @@
         <v>16</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>14</v>
@@ -3893,7 +3902,7 @@
         <v>16</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>14</v>
@@ -3910,7 +3919,7 @@
         <v>16</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>14</v>
@@ -3927,7 +3936,7 @@
         <v>16</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>14</v>
@@ -3944,12 +3953,63 @@
         <v>16</v>
       </c>
       <c r="C159" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E159" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F160" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C162" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E159" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F159" s="1" t="s">
+      <c r="E162" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F162" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3997,12 +4057,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4120,15 +4177,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4150,16 +4217,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiornamento librerie e formule
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="179">
   <si>
     <t>Action</t>
   </si>
@@ -637,6 +637,9 @@
   </si>
   <si>
     <t>INDICATOR_83</t>
+  </si>
+  <si>
+    <t>INDICATOR_36</t>
   </si>
 </sst>
 </file>
@@ -1239,10 +1242,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83:F86"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1946,8 +1949,8 @@
       <c r="B41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>33</v>
+      <c r="C41" s="5" t="s">
+        <v>178</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>14</v>
@@ -1963,8 +1966,8 @@
       <c r="B42" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>46</v>
+      <c r="C42" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>14</v>
@@ -1981,7 +1984,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>14</v>
@@ -1998,7 +2001,7 @@
         <v>16</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>14</v>
@@ -2015,7 +2018,7 @@
         <v>16</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>14</v>
@@ -2032,7 +2035,7 @@
         <v>16</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>14</v>
@@ -2049,7 +2052,7 @@
         <v>16</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>14</v>
@@ -2066,7 +2069,7 @@
         <v>16</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>14</v>
@@ -2083,7 +2086,7 @@
         <v>16</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>14</v>
@@ -2100,7 +2103,7 @@
         <v>16</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>14</v>
@@ -2117,7 +2120,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>14</v>
@@ -2134,7 +2137,7 @@
         <v>16</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>14</v>
@@ -2151,7 +2154,7 @@
         <v>16</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>14</v>
@@ -2168,7 +2171,7 @@
         <v>16</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>14</v>
@@ -2185,7 +2188,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>14</v>
@@ -2202,7 +2205,7 @@
         <v>16</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>14</v>
@@ -2219,7 +2222,7 @@
         <v>16</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>14</v>
@@ -2236,7 +2239,7 @@
         <v>16</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>14</v>
@@ -2253,7 +2256,7 @@
         <v>16</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>14</v>
@@ -2270,7 +2273,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>14</v>
@@ -2287,7 +2290,7 @@
         <v>16</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>14</v>
@@ -2304,7 +2307,7 @@
         <v>16</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>14</v>
@@ -2321,7 +2324,7 @@
         <v>16</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>14</v>
@@ -2338,7 +2341,7 @@
         <v>16</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>14</v>
@@ -2355,7 +2358,7 @@
         <v>16</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>14</v>
@@ -2372,7 +2375,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>14</v>
@@ -2389,7 +2392,7 @@
         <v>16</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>14</v>
@@ -2406,7 +2409,7 @@
         <v>16</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>14</v>
@@ -2423,7 +2426,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>14</v>
@@ -2440,7 +2443,7 @@
         <v>16</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>14</v>
@@ -2457,7 +2460,7 @@
         <v>16</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>14</v>
@@ -2474,7 +2477,7 @@
         <v>16</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>14</v>
@@ -2491,7 +2494,7 @@
         <v>16</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>14</v>
@@ -2508,7 +2511,7 @@
         <v>16</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>14</v>
@@ -2525,7 +2528,7 @@
         <v>16</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>14</v>
@@ -2542,7 +2545,7 @@
         <v>16</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>14</v>
@@ -2559,7 +2562,7 @@
         <v>16</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>14</v>
@@ -2576,7 +2579,7 @@
         <v>16</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>14</v>
@@ -2593,7 +2596,7 @@
         <v>16</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>14</v>
@@ -2610,7 +2613,7 @@
         <v>16</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>14</v>
@@ -2627,7 +2630,7 @@
         <v>16</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>14</v>
@@ -2644,7 +2647,7 @@
         <v>16</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>14</v>
@@ -2661,7 +2664,7 @@
         <v>16</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>14</v>
@@ -2678,7 +2681,7 @@
         <v>16</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>14</v>
@@ -2695,7 +2698,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>14</v>
@@ -2712,7 +2715,7 @@
         <v>16</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>14</v>
@@ -2729,7 +2732,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>14</v>
@@ -2746,7 +2749,7 @@
         <v>16</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>14</v>
@@ -2763,7 +2766,7 @@
         <v>16</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>14</v>
@@ -2780,7 +2783,7 @@
         <v>16</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>14</v>
@@ -2797,7 +2800,7 @@
         <v>16</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>14</v>
@@ -2814,7 +2817,7 @@
         <v>16</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>14</v>
@@ -2831,7 +2834,7 @@
         <v>16</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>14</v>
@@ -2848,7 +2851,7 @@
         <v>16</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>14</v>
@@ -2865,7 +2868,7 @@
         <v>16</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>14</v>
@@ -2882,7 +2885,7 @@
         <v>16</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>14</v>
@@ -2899,7 +2902,7 @@
         <v>16</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>14</v>
@@ -2916,7 +2919,7 @@
         <v>16</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>14</v>
@@ -2933,7 +2936,7 @@
         <v>16</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>14</v>
@@ -2950,7 +2953,7 @@
         <v>16</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>14</v>
@@ -2967,7 +2970,7 @@
         <v>16</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>14</v>
@@ -2984,7 +2987,7 @@
         <v>16</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>14</v>
@@ -3001,7 +3004,7 @@
         <v>16</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>14</v>
@@ -3018,7 +3021,7 @@
         <v>16</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>14</v>
@@ -3035,7 +3038,7 @@
         <v>16</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>14</v>
@@ -3052,7 +3055,7 @@
         <v>16</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>14</v>
@@ -3069,7 +3072,7 @@
         <v>16</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>14</v>
@@ -3086,7 +3089,7 @@
         <v>16</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>14</v>
@@ -3103,7 +3106,7 @@
         <v>16</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>14</v>
@@ -3120,7 +3123,7 @@
         <v>16</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>14</v>
@@ -3137,7 +3140,7 @@
         <v>16</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>14</v>
@@ -3154,7 +3157,7 @@
         <v>16</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>14</v>
@@ -3171,7 +3174,7 @@
         <v>16</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>14</v>
@@ -3188,7 +3191,7 @@
         <v>16</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>14</v>
@@ -3205,7 +3208,7 @@
         <v>16</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>14</v>
@@ -3222,7 +3225,7 @@
         <v>16</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>14</v>
@@ -3239,7 +3242,7 @@
         <v>16</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>14</v>
@@ -3256,7 +3259,7 @@
         <v>16</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>14</v>
@@ -3273,7 +3276,7 @@
         <v>16</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>14</v>
@@ -3290,7 +3293,7 @@
         <v>16</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>14</v>
@@ -3307,7 +3310,7 @@
         <v>16</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>14</v>
@@ -3324,7 +3327,7 @@
         <v>16</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>14</v>
@@ -3341,7 +3344,7 @@
         <v>16</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>14</v>
@@ -3358,7 +3361,7 @@
         <v>16</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>14</v>
@@ -3375,7 +3378,7 @@
         <v>16</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>14</v>
@@ -3392,7 +3395,7 @@
         <v>16</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>14</v>
@@ -3409,7 +3412,7 @@
         <v>16</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>14</v>
@@ -3426,7 +3429,7 @@
         <v>16</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>14</v>
@@ -3443,7 +3446,7 @@
         <v>16</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>14</v>
@@ -3460,7 +3463,7 @@
         <v>16</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>14</v>
@@ -3477,7 +3480,7 @@
         <v>16</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>14</v>
@@ -3494,7 +3497,7 @@
         <v>16</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>14</v>
@@ -3511,7 +3514,7 @@
         <v>16</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>14</v>
@@ -3528,7 +3531,7 @@
         <v>16</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>14</v>
@@ -3545,7 +3548,7 @@
         <v>16</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>14</v>
@@ -3562,7 +3565,7 @@
         <v>16</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>14</v>
@@ -3579,7 +3582,7 @@
         <v>16</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>14</v>
@@ -3596,7 +3599,7 @@
         <v>16</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>14</v>
@@ -3613,7 +3616,7 @@
         <v>16</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>14</v>
@@ -3630,7 +3633,7 @@
         <v>16</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>14</v>
@@ -3647,7 +3650,7 @@
         <v>16</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>14</v>
@@ -3664,7 +3667,7 @@
         <v>16</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>14</v>
@@ -3681,7 +3684,7 @@
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>14</v>
@@ -3698,7 +3701,7 @@
         <v>16</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>14</v>
@@ -3715,7 +3718,7 @@
         <v>16</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>14</v>
@@ -3732,7 +3735,7 @@
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>14</v>
@@ -3749,7 +3752,7 @@
         <v>16</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>14</v>
@@ -3766,7 +3769,7 @@
         <v>16</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>14</v>
@@ -3783,7 +3786,7 @@
         <v>16</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>14</v>
@@ -3800,7 +3803,7 @@
         <v>16</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>14</v>
@@ -3817,7 +3820,7 @@
         <v>16</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>14</v>
@@ -3834,7 +3837,7 @@
         <v>16</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>14</v>
@@ -3851,7 +3854,7 @@
         <v>16</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>14</v>
@@ -3868,7 +3871,7 @@
         <v>16</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>14</v>
@@ -3885,7 +3888,7 @@
         <v>16</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>14</v>
@@ -3902,7 +3905,7 @@
         <v>16</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>14</v>
@@ -3919,7 +3922,7 @@
         <v>16</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>14</v>
@@ -3936,7 +3939,7 @@
         <v>16</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>14</v>
@@ -3953,7 +3956,7 @@
         <v>16</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>14</v>
@@ -3970,7 +3973,7 @@
         <v>16</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>14</v>
@@ -3987,7 +3990,7 @@
         <v>16</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>14</v>
@@ -4004,12 +4007,29 @@
         <v>16</v>
       </c>
       <c r="C162" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F162" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C163" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E162" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F162" s="1" t="s">
+      <c r="E163" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F163" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nuovi indicatori semaforo di gruppo
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="184">
   <si>
     <t>Action</t>
   </si>
@@ -640,12 +640,27 @@
   </si>
   <si>
     <t>INDICATOR_36</t>
+  </si>
+  <si>
+    <t>INDICATOR_QUOTA_EXP_GRP1</t>
+  </si>
+  <si>
+    <t>INDICATOR_QUOTA_EXP_GRP2</t>
+  </si>
+  <si>
+    <t>INDICATOR_QUOTA_EXP_GRP3</t>
+  </si>
+  <si>
+    <t>SEMAFORO_DI_GRUPPO</t>
+  </si>
+  <si>
+    <t>CALCOLO_MODULO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1242,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G163"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -4030,6 +4045,91 @@
         <v>14</v>
       </c>
       <c r="F163" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E165" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E166" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F168" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4077,9 +4177,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4197,25 +4300,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4237,9 +4330,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ADD:  - Moduli  - Semaforo di gruppo  - FIX Formule BASE
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -654,9 +654,6 @@
     <t>SEMAFORO_DI_GRUPPO</t>
   </si>
   <si>
-    <t>CALCOLO_MODULO</t>
-  </si>
-  <si>
     <t>INDICATOR_37</t>
   </si>
   <si>
@@ -676,12 +673,15 @@
   </si>
   <si>
     <t>INDICATOR_43</t>
+  </si>
+  <si>
+    <t>getAllModulesElaboration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2020,7 +2020,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>14</v>
@@ -2037,7 +2037,7 @@
         <v>16</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>14</v>
@@ -2054,7 +2054,7 @@
         <v>16</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>14</v>
@@ -2071,7 +2071,7 @@
         <v>16</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>14</v>
@@ -2088,7 +2088,7 @@
         <v>16</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>14</v>
@@ -2105,7 +2105,7 @@
         <v>16</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>14</v>
@@ -2122,7 +2122,7 @@
         <v>16</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>14</v>
@@ -4247,7 +4247,7 @@
         <v>16</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>14</v>
@@ -4431,18 +4431,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4462,14 +4462,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4482,4 +4474,12 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiunti colore assi matrice VM
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="192">
   <si>
     <t>Action</t>
   </si>
@@ -676,6 +676,9 @@
   </si>
   <si>
     <t>getAllModulesElaboration</t>
+  </si>
+  <si>
+    <t>getMatrixAxis</t>
   </si>
 </sst>
 </file>
@@ -1278,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:G176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C174" sqref="C174"/>
+      <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -4270,6 +4273,23 @@
         <v>14</v>
       </c>
       <c r="F175" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F176" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4317,6 +4337,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -4430,33 +4465,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4477,9 +4489,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiornamento ind test aqr
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="199">
   <si>
     <t>Action</t>
   </si>
@@ -691,6 +691,15 @@
   </si>
   <si>
     <t>INDICATOR_87</t>
+  </si>
+  <si>
+    <t>IND_12_CHANGE</t>
+  </si>
+  <si>
+    <t>IND_12_DELTA_DT</t>
+  </si>
+  <si>
+    <t>IND_212_FL_OVERRIDE</t>
   </si>
 </sst>
 </file>
@@ -744,7 +753,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -754,6 +763,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFAC2524"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -769,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -778,6 +793,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1293,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94:F98"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2334,53 +2352,56 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F61" s="1" t="s">
+      <c r="A61" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D61" s="8"/>
+      <c r="E61" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F62" s="1" t="s">
+      <c r="A62" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D62" s="8"/>
+      <c r="E62" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F63" s="1" t="s">
+      <c r="A63" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D63" s="8"/>
+      <c r="E63" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2392,7 +2413,7 @@
         <v>16</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>14</v>
@@ -2409,7 +2430,7 @@
         <v>16</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>14</v>
@@ -2426,7 +2447,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>14</v>
@@ -2443,7 +2464,7 @@
         <v>16</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>14</v>
@@ -2460,7 +2481,7 @@
         <v>16</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>14</v>
@@ -2477,7 +2498,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>14</v>
@@ -2494,7 +2515,7 @@
         <v>16</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>14</v>
@@ -2511,7 +2532,7 @@
         <v>16</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>14</v>
@@ -2528,7 +2549,7 @@
         <v>16</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>14</v>
@@ -2545,7 +2566,7 @@
         <v>16</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>14</v>
@@ -2562,7 +2583,7 @@
         <v>16</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>14</v>
@@ -2579,7 +2600,7 @@
         <v>16</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>14</v>
@@ -2596,7 +2617,7 @@
         <v>16</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>14</v>
@@ -2613,7 +2634,7 @@
         <v>16</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>14</v>
@@ -2630,7 +2651,7 @@
         <v>16</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>14</v>
@@ -2647,7 +2668,7 @@
         <v>16</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>14</v>
@@ -2664,7 +2685,7 @@
         <v>16</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>14</v>
@@ -2681,7 +2702,7 @@
         <v>16</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>14</v>
@@ -2698,7 +2719,7 @@
         <v>16</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>14</v>
@@ -2715,7 +2736,7 @@
         <v>16</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>14</v>
@@ -2732,7 +2753,7 @@
         <v>16</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>14</v>
@@ -2749,7 +2770,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>14</v>
@@ -2766,7 +2787,7 @@
         <v>16</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>14</v>
@@ -2783,7 +2804,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>14</v>
@@ -2800,7 +2821,7 @@
         <v>16</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>14</v>
@@ -2817,7 +2838,7 @@
         <v>16</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>14</v>
@@ -2834,7 +2855,7 @@
         <v>16</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>14</v>
@@ -2851,7 +2872,7 @@
         <v>16</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>14</v>
@@ -2868,7 +2889,7 @@
         <v>16</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>175</v>
+        <v>122</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>14</v>
@@ -2885,7 +2906,7 @@
         <v>16</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>176</v>
+        <v>123</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>14</v>
@@ -2902,7 +2923,7 @@
         <v>16</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>177</v>
+        <v>124</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>14</v>
@@ -2919,7 +2940,7 @@
         <v>16</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>14</v>
@@ -2936,7 +2957,7 @@
         <v>16</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>14</v>
@@ -2953,7 +2974,7 @@
         <v>16</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>14</v>
@@ -2970,7 +2991,7 @@
         <v>16</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>14</v>
@@ -2987,7 +3008,7 @@
         <v>16</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>62</v>
+        <v>193</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>14</v>
@@ -3004,7 +3025,7 @@
         <v>16</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>63</v>
+        <v>194</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>14</v>
@@ -3021,7 +3042,7 @@
         <v>16</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>64</v>
+        <v>195</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>14</v>
@@ -3038,7 +3059,7 @@
         <v>16</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>14</v>
@@ -3055,7 +3076,7 @@
         <v>16</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>14</v>
@@ -3072,7 +3093,7 @@
         <v>16</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>14</v>
@@ -3089,7 +3110,7 @@
         <v>16</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>14</v>
@@ -3106,7 +3127,7 @@
         <v>16</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>14</v>
@@ -3123,7 +3144,7 @@
         <v>16</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>14</v>
@@ -3140,7 +3161,7 @@
         <v>16</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>14</v>
@@ -3157,7 +3178,7 @@
         <v>16</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>14</v>
@@ -3174,7 +3195,7 @@
         <v>16</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>14</v>
@@ -3191,7 +3212,7 @@
         <v>16</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>14</v>
@@ -3208,7 +3229,7 @@
         <v>16</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>14</v>
@@ -3225,7 +3246,7 @@
         <v>16</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>14</v>
@@ -3242,7 +3263,7 @@
         <v>16</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>14</v>
@@ -3259,7 +3280,7 @@
         <v>16</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>14</v>
@@ -3276,7 +3297,7 @@
         <v>16</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>14</v>
@@ -3293,7 +3314,7 @@
         <v>16</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>14</v>
@@ -3310,7 +3331,7 @@
         <v>16</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>14</v>
@@ -3327,7 +3348,7 @@
         <v>16</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>14</v>
@@ -3344,7 +3365,7 @@
         <v>16</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>14</v>
@@ -3361,7 +3382,7 @@
         <v>16</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>14</v>
@@ -3378,7 +3399,7 @@
         <v>16</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>14</v>
@@ -3395,7 +3416,7 @@
         <v>16</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>14</v>
@@ -3412,7 +3433,7 @@
         <v>16</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>14</v>
@@ -3429,7 +3450,7 @@
         <v>16</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>14</v>
@@ -3446,7 +3467,7 @@
         <v>16</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>14</v>
@@ -3463,7 +3484,7 @@
         <v>16</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>14</v>
@@ -3480,7 +3501,7 @@
         <v>16</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>14</v>
@@ -3497,7 +3518,7 @@
         <v>16</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>14</v>
@@ -3514,7 +3535,7 @@
         <v>16</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>14</v>
@@ -3531,7 +3552,7 @@
         <v>16</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>14</v>
@@ -3548,7 +3569,7 @@
         <v>16</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>14</v>
@@ -3565,7 +3586,7 @@
         <v>16</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>14</v>
@@ -3582,7 +3603,7 @@
         <v>16</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>14</v>
@@ -3599,7 +3620,7 @@
         <v>16</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>14</v>
@@ -3616,7 +3637,7 @@
         <v>16</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>14</v>
@@ -3633,7 +3654,7 @@
         <v>16</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>14</v>
@@ -3650,7 +3671,7 @@
         <v>16</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>14</v>
@@ -3667,7 +3688,7 @@
         <v>16</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>14</v>
@@ -3684,7 +3705,7 @@
         <v>16</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>14</v>
@@ -3701,7 +3722,7 @@
         <v>16</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>14</v>
@@ -3718,7 +3739,7 @@
         <v>16</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>14</v>
@@ -3735,7 +3756,7 @@
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>14</v>
@@ -3752,7 +3773,7 @@
         <v>16</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>14</v>
@@ -3769,7 +3790,7 @@
         <v>16</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>14</v>
@@ -3786,7 +3807,7 @@
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>14</v>
@@ -3803,7 +3824,7 @@
         <v>16</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>14</v>
@@ -3820,7 +3841,7 @@
         <v>16</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>14</v>
@@ -3837,7 +3858,7 @@
         <v>16</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>14</v>
@@ -3854,7 +3875,7 @@
         <v>16</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>14</v>
@@ -3871,7 +3892,7 @@
         <v>16</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>14</v>
@@ -3888,7 +3909,7 @@
         <v>16</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>14</v>
@@ -3905,7 +3926,7 @@
         <v>16</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>14</v>
@@ -3922,7 +3943,7 @@
         <v>16</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>14</v>
@@ -3939,7 +3960,7 @@
         <v>16</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>14</v>
@@ -3956,7 +3977,7 @@
         <v>16</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>14</v>
@@ -3973,7 +3994,7 @@
         <v>16</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>14</v>
@@ -3990,7 +4011,7 @@
         <v>16</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>14</v>
@@ -4007,7 +4028,7 @@
         <v>16</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>14</v>
@@ -4024,7 +4045,7 @@
         <v>16</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>14</v>
@@ -4041,7 +4062,7 @@
         <v>16</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>14</v>
@@ -4058,7 +4079,7 @@
         <v>16</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>14</v>
@@ -4075,7 +4096,7 @@
         <v>16</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>14</v>
@@ -4092,7 +4113,7 @@
         <v>16</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>14</v>
@@ -4109,7 +4130,7 @@
         <v>16</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>14</v>
@@ -4126,7 +4147,7 @@
         <v>16</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>14</v>
@@ -4143,7 +4164,7 @@
         <v>16</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>14</v>
@@ -4160,7 +4181,7 @@
         <v>16</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>14</v>
@@ -4177,7 +4198,7 @@
         <v>16</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>14</v>
@@ -4194,7 +4215,7 @@
         <v>16</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>14</v>
@@ -4211,7 +4232,7 @@
         <v>16</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>14</v>
@@ -4228,7 +4249,7 @@
         <v>16</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>14</v>
@@ -4245,7 +4266,7 @@
         <v>16</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>14</v>
@@ -4262,7 +4283,7 @@
         <v>16</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>14</v>
@@ -4278,8 +4299,8 @@
       <c r="B175" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C175" s="3" t="s">
-        <v>179</v>
+      <c r="C175" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>14</v>
@@ -4295,8 +4316,8 @@
       <c r="B176" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C176" s="3" t="s">
-        <v>180</v>
+      <c r="C176" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>14</v>
@@ -4312,8 +4333,8 @@
       <c r="B177" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C177" s="3" t="s">
-        <v>181</v>
+      <c r="C177" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>14</v>
@@ -4329,8 +4350,8 @@
       <c r="B178" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C178" s="1" t="s">
-        <v>190</v>
+      <c r="C178" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>14</v>
@@ -4347,7 +4368,7 @@
         <v>16</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>14</v>
@@ -4363,13 +4384,64 @@
       <c r="B180" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C180" s="1" t="s">
+      <c r="C180" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F181" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A182" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A183" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C183" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E180" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F180" s="1" t="s">
+      <c r="E183" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F183" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4417,6 +4489,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -4530,33 +4617,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4577,9 +4641,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
nuovi indicatori override NOPG - 25,525,512, 36, 536, FITCH
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Library_Formula" sheetId="2" r:id="rId2"/>
     <sheet name="Formula Libraries Labels" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="234">
   <si>
     <t>Action</t>
   </si>
@@ -712,6 +712,99 @@
   </si>
   <si>
     <t>IND_118_FL_SUPER</t>
+  </si>
+  <si>
+    <t>IND_25_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_525_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_512_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_25_OVER</t>
+  </si>
+  <si>
+    <t>IND_525_OVER</t>
+  </si>
+  <si>
+    <t>IND_512_OVER</t>
+  </si>
+  <si>
+    <t>IND_36_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_536_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_36_SUPER</t>
+  </si>
+  <si>
+    <t>IND_132_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_133_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_134_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_135_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_136_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_137_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_138_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_139_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_140_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_141_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_142_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_132_OVER</t>
+  </si>
+  <si>
+    <t>IND_133_OVER</t>
+  </si>
+  <si>
+    <t>IND_134_OVER</t>
+  </si>
+  <si>
+    <t>IND_135_FL_DATE_12M</t>
+  </si>
+  <si>
+    <t>IND_136_OVER</t>
+  </si>
+  <si>
+    <t>IND_137_OVER</t>
+  </si>
+  <si>
+    <t>IND_138_OVER</t>
+  </si>
+  <si>
+    <t>IND_139_OVER</t>
+  </si>
+  <si>
+    <t>IND_140_OVER</t>
+  </si>
+  <si>
+    <t>IND_141_OVER</t>
+  </si>
+  <si>
+    <t>IND_142_OVER</t>
   </si>
 </sst>
 </file>
@@ -1323,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G187"/>
+  <dimension ref="A1:G218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2385,53 +2478,56 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F62" s="1" t="s">
+      <c r="A62" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D62" s="8"/>
+      <c r="E62" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F63" s="1" t="s">
+      <c r="A63" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D63" s="8"/>
+      <c r="E63" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F63" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F64" s="1" t="s">
+      <c r="A64" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F64" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2443,7 +2539,7 @@
         <v>16</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="7" t="s">
@@ -2461,7 +2557,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="7" t="s">
@@ -2479,7 +2575,7 @@
         <v>16</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="7" t="s">
@@ -2490,439 +2586,464 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F68" s="1" t="s">
+      <c r="A68" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D68" s="8"/>
+      <c r="E68" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F69" s="1" t="s">
+      <c r="A69" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D69" s="8"/>
+      <c r="E69" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F70" s="1" t="s">
+      <c r="A70" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D70" s="8"/>
+      <c r="E70" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F71" s="1" t="s">
+      <c r="A71" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="D71" s="8"/>
+      <c r="E71" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" s="1" t="s">
+      <c r="A72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D72" s="8"/>
+      <c r="E72" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" s="1" t="s">
+      <c r="A73" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D73" s="8"/>
+      <c r="E73" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F74" s="1" t="s">
+      <c r="A74" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D74" s="8"/>
+      <c r="E74" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F74" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F75" s="1" t="s">
+      <c r="A75" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D75" s="8"/>
+      <c r="E75" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F76" s="1" t="s">
+      <c r="A76" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D76" s="8"/>
+      <c r="E76" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77" s="1" t="s">
+      <c r="A77" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D77" s="8"/>
+      <c r="E77" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F78" s="1" t="s">
+      <c r="A78" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D78" s="8"/>
+      <c r="E78" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F78" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F79" s="1" t="s">
+      <c r="A79" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D79" s="8"/>
+      <c r="E79" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F80" s="1" t="s">
+      <c r="A80" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D80" s="8"/>
+      <c r="E80" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F80" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F81" s="1" t="s">
+      <c r="A81" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D81" s="8"/>
+      <c r="E81" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F81" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F82" s="1" t="s">
+      <c r="A82" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D82" s="8"/>
+      <c r="E82" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F83" s="1" t="s">
+      <c r="A83" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D83" s="8"/>
+      <c r="E83" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F84" s="1" t="s">
+      <c r="A84" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D84" s="8"/>
+      <c r="E84" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F85" s="1" t="s">
+      <c r="A85" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D85" s="8"/>
+      <c r="E85" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F86" s="1" t="s">
+      <c r="A86" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D86" s="8"/>
+      <c r="E86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F86" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F87" s="1" t="s">
+      <c r="A87" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D87" s="8"/>
+      <c r="E87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F87" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F88" s="1" t="s">
+      <c r="A88" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D88" s="8"/>
+      <c r="E88" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F89" s="1" t="s">
+      <c r="A89" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D89" s="8"/>
+      <c r="E89" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F89" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F90" s="1" t="s">
+      <c r="A90" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D90" s="8"/>
+      <c r="E90" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F90" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F91" s="1" t="s">
+      <c r="A91" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D91" s="8"/>
+      <c r="E91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F92" s="1" t="s">
+      <c r="A92" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D92" s="8"/>
+      <c r="E92" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B93" s="1" t="s">
+      <c r="A93" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>119</v>
+        <v>53</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>14</v>
@@ -2939,7 +3060,7 @@
         <v>16</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>14</v>
@@ -2956,7 +3077,7 @@
         <v>16</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>121</v>
+        <v>56</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>14</v>
@@ -2966,53 +3087,56 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96" s="1" t="s">
+      <c r="A96" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D96" s="8"/>
+      <c r="E96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F97" s="1" t="s">
+      <c r="A97" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D97" s="8"/>
+      <c r="E97" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E98" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F98" s="1" t="s">
+      <c r="A98" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D98" s="8"/>
+      <c r="E98" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F98" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3024,7 +3148,7 @@
         <v>16</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>175</v>
+        <v>57</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>14</v>
@@ -3041,7 +3165,7 @@
         <v>16</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>176</v>
+        <v>58</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>14</v>
@@ -3058,7 +3182,7 @@
         <v>16</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>177</v>
+        <v>59</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>14</v>
@@ -3075,7 +3199,7 @@
         <v>16</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>192</v>
+        <v>60</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>14</v>
@@ -3092,7 +3216,7 @@
         <v>16</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>193</v>
+        <v>61</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>14</v>
@@ -3109,7 +3233,7 @@
         <v>16</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>194</v>
+        <v>68</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>14</v>
@@ -3126,7 +3250,7 @@
         <v>16</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>195</v>
+        <v>69</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>14</v>
@@ -3143,7 +3267,7 @@
         <v>16</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>14</v>
@@ -3160,7 +3284,7 @@
         <v>16</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>14</v>
@@ -3177,7 +3301,7 @@
         <v>16</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>14</v>
@@ -3194,7 +3318,7 @@
         <v>16</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>14</v>
@@ -3211,7 +3335,7 @@
         <v>16</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>14</v>
@@ -3228,7 +3352,7 @@
         <v>16</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>14</v>
@@ -3245,7 +3369,7 @@
         <v>16</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>14</v>
@@ -3262,7 +3386,7 @@
         <v>16</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>14</v>
@@ -3279,7 +3403,7 @@
         <v>16</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>14</v>
@@ -3296,7 +3420,7 @@
         <v>16</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>14</v>
@@ -3313,7 +3437,7 @@
         <v>16</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>14</v>
@@ -3330,7 +3454,7 @@
         <v>16</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>14</v>
@@ -3347,7 +3471,7 @@
         <v>16</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>14</v>
@@ -3364,7 +3488,7 @@
         <v>16</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>14</v>
@@ -3381,7 +3505,7 @@
         <v>16</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>14</v>
@@ -3398,7 +3522,7 @@
         <v>16</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>14</v>
@@ -3415,7 +3539,7 @@
         <v>16</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>84</v>
+        <v>117</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>14</v>
@@ -3432,7 +3556,7 @@
         <v>16</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>14</v>
@@ -3449,7 +3573,7 @@
         <v>16</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>86</v>
+        <v>119</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>14</v>
@@ -3466,7 +3590,7 @@
         <v>16</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>14</v>
@@ -3483,7 +3607,7 @@
         <v>16</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>88</v>
+        <v>121</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>14</v>
@@ -3500,7 +3624,7 @@
         <v>16</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>14</v>
@@ -3517,7 +3641,7 @@
         <v>16</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>14</v>
@@ -3534,7 +3658,7 @@
         <v>16</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>14</v>
@@ -3551,7 +3675,7 @@
         <v>16</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>92</v>
+        <v>175</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>14</v>
@@ -3568,7 +3692,7 @@
         <v>16</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>14</v>
@@ -3585,7 +3709,7 @@
         <v>16</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>14</v>
@@ -3602,7 +3726,7 @@
         <v>16</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>95</v>
+        <v>192</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>14</v>
@@ -3619,7 +3743,7 @@
         <v>16</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>14</v>
@@ -3636,7 +3760,7 @@
         <v>16</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>97</v>
+        <v>194</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>14</v>
@@ -3653,7 +3777,7 @@
         <v>16</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>14</v>
@@ -3670,7 +3794,7 @@
         <v>16</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>99</v>
+        <v>62</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>14</v>
@@ -3687,7 +3811,7 @@
         <v>16</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>14</v>
@@ -3704,7 +3828,7 @@
         <v>16</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>14</v>
@@ -3721,7 +3845,7 @@
         <v>16</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>14</v>
@@ -3738,7 +3862,7 @@
         <v>16</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>14</v>
@@ -3755,7 +3879,7 @@
         <v>16</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>14</v>
@@ -3772,7 +3896,7 @@
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>14</v>
@@ -3789,7 +3913,7 @@
         <v>16</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>14</v>
@@ -3806,7 +3930,7 @@
         <v>16</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>14</v>
@@ -3823,7 +3947,7 @@
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>14</v>
@@ -3840,7 +3964,7 @@
         <v>16</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>14</v>
@@ -3857,7 +3981,7 @@
         <v>16</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>14</v>
@@ -3874,7 +3998,7 @@
         <v>16</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>14</v>
@@ -3891,7 +4015,7 @@
         <v>16</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>14</v>
@@ -3908,7 +4032,7 @@
         <v>16</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>14</v>
@@ -3925,7 +4049,7 @@
         <v>16</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>14</v>
@@ -3942,7 +4066,7 @@
         <v>16</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>14</v>
@@ -3959,7 +4083,7 @@
         <v>16</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>14</v>
@@ -3976,7 +4100,7 @@
         <v>16</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>14</v>
@@ -3993,7 +4117,7 @@
         <v>16</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>14</v>
@@ -4010,7 +4134,7 @@
         <v>16</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>14</v>
@@ -4027,7 +4151,7 @@
         <v>16</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>14</v>
@@ -4044,7 +4168,7 @@
         <v>16</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>14</v>
@@ -4061,7 +4185,7 @@
         <v>16</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>14</v>
@@ -4078,7 +4202,7 @@
         <v>16</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>14</v>
@@ -4095,7 +4219,7 @@
         <v>16</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>14</v>
@@ -4112,7 +4236,7 @@
         <v>16</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>14</v>
@@ -4129,7 +4253,7 @@
         <v>16</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>14</v>
@@ -4146,7 +4270,7 @@
         <v>16</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>14</v>
@@ -4163,7 +4287,7 @@
         <v>16</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>148</v>
+        <v>97</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>14</v>
@@ -4180,7 +4304,7 @@
         <v>16</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>14</v>
@@ -4197,7 +4321,7 @@
         <v>16</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>14</v>
@@ -4214,7 +4338,7 @@
         <v>16</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>14</v>
@@ -4231,7 +4355,7 @@
         <v>16</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>14</v>
@@ -4248,7 +4372,7 @@
         <v>16</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>14</v>
@@ -4265,7 +4389,7 @@
         <v>16</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>14</v>
@@ -4282,7 +4406,7 @@
         <v>16</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>14</v>
@@ -4299,7 +4423,7 @@
         <v>16</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>14</v>
@@ -4316,7 +4440,7 @@
         <v>16</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>14</v>
@@ -4333,7 +4457,7 @@
         <v>16</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>14</v>
@@ -4350,7 +4474,7 @@
         <v>16</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>14</v>
@@ -4367,7 +4491,7 @@
         <v>16</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>14</v>
@@ -4384,7 +4508,7 @@
         <v>16</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>14</v>
@@ -4401,7 +4525,7 @@
         <v>16</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>14</v>
@@ -4418,7 +4542,7 @@
         <v>16</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>14</v>
@@ -4434,8 +4558,8 @@
       <c r="B182" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C182" s="3" t="s">
-        <v>179</v>
+      <c r="C182" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>14</v>
@@ -4451,8 +4575,8 @@
       <c r="B183" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C183" s="3" t="s">
-        <v>180</v>
+      <c r="C183" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>14</v>
@@ -4468,8 +4592,8 @@
       <c r="B184" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C184" s="3" t="s">
-        <v>181</v>
+      <c r="C184" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>14</v>
@@ -4486,7 +4610,7 @@
         <v>16</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>190</v>
+        <v>136</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>14</v>
@@ -4502,8 +4626,8 @@
       <c r="B186" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C186" s="3" t="s">
-        <v>182</v>
+      <c r="C186" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>14</v>
@@ -4520,12 +4644,539 @@
         <v>16</v>
       </c>
       <c r="C187" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F187" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A190" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A192" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A195" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A197" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A198" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A199" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F200" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A202" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A204" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A205" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A206" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E206" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F206" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A207" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A208" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F208" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A209" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A210" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F210" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A211" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A212" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F212" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A213" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F213" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A214" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F214" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A215" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F215" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A216" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A217" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F217" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A218" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C218" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E187" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F187" s="1" t="s">
+      <c r="E218" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F218" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4573,18 +5224,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4702,14 +5353,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4720,6 +5363,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
AGGIORNAMENTO STATIC E TEST ALEX SVIL/SIT
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="236">
   <si>
     <t>Action</t>
   </si>
@@ -805,6 +805,12 @@
   </si>
   <si>
     <t>IND_142_OVER</t>
+  </si>
+  <si>
+    <t>IND_37_FL_OVERRIDE</t>
+  </si>
+  <si>
+    <t>IND_37_SUPER</t>
   </si>
 </sst>
 </file>
@@ -1416,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G218"/>
+  <dimension ref="A1:G220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2485,7 +2491,7 @@
         <v>16</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>203</v>
+        <v>234</v>
       </c>
       <c r="D62" s="8"/>
       <c r="E62" s="7" t="s">
@@ -2503,7 +2509,7 @@
         <v>16</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="7" t="s">
@@ -2521,7 +2527,7 @@
         <v>16</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D64" s="8"/>
       <c r="E64" s="7" t="s">
@@ -2539,7 +2545,7 @@
         <v>16</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="7" t="s">
@@ -2557,7 +2563,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="7" t="s">
@@ -2575,7 +2581,7 @@
         <v>16</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="7" t="s">
@@ -2593,7 +2599,7 @@
         <v>16</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D68" s="8"/>
       <c r="E68" s="7" t="s">
@@ -2611,7 +2617,7 @@
         <v>16</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D69" s="8"/>
       <c r="E69" s="7" t="s">
@@ -2629,7 +2635,7 @@
         <v>16</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="7" t="s">
@@ -2647,7 +2653,7 @@
         <v>16</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="7" t="s">
@@ -2665,7 +2671,7 @@
         <v>16</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D72" s="8"/>
       <c r="E72" s="7" t="s">
@@ -2683,7 +2689,7 @@
         <v>16</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D73" s="8"/>
       <c r="E73" s="7" t="s">
@@ -2701,7 +2707,7 @@
         <v>16</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D74" s="8"/>
       <c r="E74" s="7" t="s">
@@ -2719,7 +2725,7 @@
         <v>16</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D75" s="8"/>
       <c r="E75" s="7" t="s">
@@ -2737,7 +2743,7 @@
         <v>16</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D76" s="8"/>
       <c r="E76" s="7" t="s">
@@ -2755,7 +2761,7 @@
         <v>16</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D77" s="8"/>
       <c r="E77" s="7" t="s">
@@ -2773,7 +2779,7 @@
         <v>16</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D78" s="8"/>
       <c r="E78" s="7" t="s">
@@ -2791,7 +2797,7 @@
         <v>16</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D79" s="8"/>
       <c r="E79" s="7" t="s">
@@ -2809,7 +2815,7 @@
         <v>16</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D80" s="8"/>
       <c r="E80" s="7" t="s">
@@ -2827,7 +2833,7 @@
         <v>16</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D81" s="8"/>
       <c r="E81" s="7" t="s">
@@ -2845,7 +2851,7 @@
         <v>16</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="7" t="s">
@@ -2863,7 +2869,7 @@
         <v>16</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D83" s="8"/>
       <c r="E83" s="7" t="s">
@@ -2881,7 +2887,7 @@
         <v>16</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="7" t="s">
@@ -2899,7 +2905,7 @@
         <v>16</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="7" t="s">
@@ -2917,7 +2923,7 @@
         <v>16</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="7" t="s">
@@ -2935,7 +2941,7 @@
         <v>16</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D87" s="8"/>
       <c r="E87" s="7" t="s">
@@ -2953,7 +2959,7 @@
         <v>16</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="7" t="s">
@@ -2971,7 +2977,7 @@
         <v>16</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="7" t="s">
@@ -2989,7 +2995,7 @@
         <v>16</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="7" t="s">
@@ -3007,7 +3013,7 @@
         <v>16</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="7" t="s">
@@ -3025,7 +3031,7 @@
         <v>16</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D92" s="8"/>
       <c r="E92" s="7" t="s">
@@ -3042,83 +3048,83 @@
       <c r="B93" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="D93" s="8"/>
+      <c r="E93" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="D94" s="8"/>
+      <c r="E94" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C94" s="1" t="s">
+      <c r="E95" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E94" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C95" s="1" t="s">
+      <c r="E96" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D96" s="8"/>
-      <c r="E96" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D97" s="8"/>
-      <c r="E97" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F97" s="7" t="s">
+      <c r="E97" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3130,7 +3136,7 @@
         <v>16</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="7" t="s">
@@ -3141,36 +3147,38 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F99" s="1" t="s">
+      <c r="A99" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D99" s="8"/>
+      <c r="E99" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F99" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F100" s="1" t="s">
+      <c r="A100" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D100" s="8"/>
+      <c r="E100" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3182,7 +3190,7 @@
         <v>16</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>14</v>
@@ -3199,7 +3207,7 @@
         <v>16</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>14</v>
@@ -3216,7 +3224,7 @@
         <v>16</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>14</v>
@@ -3233,7 +3241,7 @@
         <v>16</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>14</v>
@@ -3250,7 +3258,7 @@
         <v>16</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>14</v>
@@ -3267,7 +3275,7 @@
         <v>16</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>14</v>
@@ -3284,7 +3292,7 @@
         <v>16</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>14</v>
@@ -3301,7 +3309,7 @@
         <v>16</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>14</v>
@@ -3318,7 +3326,7 @@
         <v>16</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>14</v>
@@ -3335,7 +3343,7 @@
         <v>16</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>14</v>
@@ -3352,7 +3360,7 @@
         <v>16</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="E111" s="1" t="s">
         <v>14</v>
@@ -3369,7 +3377,7 @@
         <v>16</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>14</v>
@@ -3386,7 +3394,7 @@
         <v>16</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>14</v>
@@ -3403,7 +3411,7 @@
         <v>16</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>14</v>
@@ -3420,7 +3428,7 @@
         <v>16</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>14</v>
@@ -3437,7 +3445,7 @@
         <v>16</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>14</v>
@@ -3454,7 +3462,7 @@
         <v>16</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>14</v>
@@ -3471,7 +3479,7 @@
         <v>16</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>14</v>
@@ -3488,7 +3496,7 @@
         <v>16</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>14</v>
@@ -3505,7 +3513,7 @@
         <v>16</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>14</v>
@@ -3522,7 +3530,7 @@
         <v>16</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>14</v>
@@ -3539,7 +3547,7 @@
         <v>16</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>14</v>
@@ -3556,7 +3564,7 @@
         <v>16</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>14</v>
@@ -3573,7 +3581,7 @@
         <v>16</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>14</v>
@@ -3590,7 +3598,7 @@
         <v>16</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>14</v>
@@ -3607,7 +3615,7 @@
         <v>16</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>14</v>
@@ -3624,7 +3632,7 @@
         <v>16</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>14</v>
@@ -3641,7 +3649,7 @@
         <v>16</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>14</v>
@@ -3658,7 +3666,7 @@
         <v>16</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>14</v>
@@ -3675,7 +3683,7 @@
         <v>16</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>14</v>
@@ -3692,7 +3700,7 @@
         <v>16</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>14</v>
@@ -3709,7 +3717,7 @@
         <v>16</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>14</v>
@@ -3726,7 +3734,7 @@
         <v>16</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>14</v>
@@ -3743,7 +3751,7 @@
         <v>16</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>14</v>
@@ -3760,7 +3768,7 @@
         <v>16</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>14</v>
@@ -3777,7 +3785,7 @@
         <v>16</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>14</v>
@@ -3794,7 +3802,7 @@
         <v>16</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>62</v>
+        <v>194</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>14</v>
@@ -3811,7 +3819,7 @@
         <v>16</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>63</v>
+        <v>195</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>14</v>
@@ -3828,7 +3836,7 @@
         <v>16</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>14</v>
@@ -3845,7 +3853,7 @@
         <v>16</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>14</v>
@@ -3862,7 +3870,7 @@
         <v>16</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>14</v>
@@ -3879,7 +3887,7 @@
         <v>16</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>14</v>
@@ -3896,7 +3904,7 @@
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>14</v>
@@ -3913,7 +3921,7 @@
         <v>16</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>14</v>
@@ -3930,7 +3938,7 @@
         <v>16</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>14</v>
@@ -3947,7 +3955,7 @@
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>14</v>
@@ -3964,7 +3972,7 @@
         <v>16</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>14</v>
@@ -3981,7 +3989,7 @@
         <v>16</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>14</v>
@@ -3998,7 +4006,7 @@
         <v>16</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>14</v>
@@ -4015,7 +4023,7 @@
         <v>16</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>14</v>
@@ -4032,7 +4040,7 @@
         <v>16</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>14</v>
@@ -4049,7 +4057,7 @@
         <v>16</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>14</v>
@@ -4066,7 +4074,7 @@
         <v>16</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>14</v>
@@ -4083,7 +4091,7 @@
         <v>16</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>14</v>
@@ -4100,7 +4108,7 @@
         <v>16</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>14</v>
@@ -4117,7 +4125,7 @@
         <v>16</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>14</v>
@@ -4134,7 +4142,7 @@
         <v>16</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>14</v>
@@ -4151,7 +4159,7 @@
         <v>16</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>14</v>
@@ -4168,7 +4176,7 @@
         <v>16</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>14</v>
@@ -4185,7 +4193,7 @@
         <v>16</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>14</v>
@@ -4202,7 +4210,7 @@
         <v>16</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>14</v>
@@ -4219,7 +4227,7 @@
         <v>16</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>14</v>
@@ -4236,7 +4244,7 @@
         <v>16</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>14</v>
@@ -4253,7 +4261,7 @@
         <v>16</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>14</v>
@@ -4270,7 +4278,7 @@
         <v>16</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>14</v>
@@ -4287,7 +4295,7 @@
         <v>16</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>14</v>
@@ -4304,7 +4312,7 @@
         <v>16</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>14</v>
@@ -4321,7 +4329,7 @@
         <v>16</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>14</v>
@@ -4338,7 +4346,7 @@
         <v>16</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>14</v>
@@ -4355,7 +4363,7 @@
         <v>16</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>14</v>
@@ -4372,7 +4380,7 @@
         <v>16</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>14</v>
@@ -4389,7 +4397,7 @@
         <v>16</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>14</v>
@@ -4406,7 +4414,7 @@
         <v>16</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>14</v>
@@ -4423,7 +4431,7 @@
         <v>16</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>14</v>
@@ -4440,7 +4448,7 @@
         <v>16</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>14</v>
@@ -4457,7 +4465,7 @@
         <v>16</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>14</v>
@@ -4474,7 +4482,7 @@
         <v>16</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>14</v>
@@ -4491,7 +4499,7 @@
         <v>16</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>14</v>
@@ -4508,7 +4516,7 @@
         <v>16</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>14</v>
@@ -4525,7 +4533,7 @@
         <v>16</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>14</v>
@@ -4542,7 +4550,7 @@
         <v>16</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>14</v>
@@ -4559,7 +4567,7 @@
         <v>16</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>14</v>
@@ -4576,7 +4584,7 @@
         <v>16</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>14</v>
@@ -4593,7 +4601,7 @@
         <v>16</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>14</v>
@@ -4610,7 +4618,7 @@
         <v>16</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>14</v>
@@ -4627,7 +4635,7 @@
         <v>16</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>14</v>
@@ -4644,7 +4652,7 @@
         <v>16</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>14</v>
@@ -4661,7 +4669,7 @@
         <v>16</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>14</v>
@@ -4678,7 +4686,7 @@
         <v>16</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>14</v>
@@ -4695,7 +4703,7 @@
         <v>16</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>14</v>
@@ -4712,7 +4720,7 @@
         <v>16</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>14</v>
@@ -4729,7 +4737,7 @@
         <v>16</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>14</v>
@@ -4746,7 +4754,7 @@
         <v>16</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>14</v>
@@ -4763,7 +4771,7 @@
         <v>16</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>14</v>
@@ -4780,7 +4788,7 @@
         <v>16</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>14</v>
@@ -4797,7 +4805,7 @@
         <v>16</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>14</v>
@@ -4814,7 +4822,7 @@
         <v>16</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>14</v>
@@ -4831,7 +4839,7 @@
         <v>16</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>14</v>
@@ -4848,7 +4856,7 @@
         <v>16</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>14</v>
@@ -4865,7 +4873,7 @@
         <v>16</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>14</v>
@@ -4882,7 +4890,7 @@
         <v>16</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>14</v>
@@ -4899,7 +4907,7 @@
         <v>16</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>14</v>
@@ -4916,7 +4924,7 @@
         <v>16</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>14</v>
@@ -4933,7 +4941,7 @@
         <v>16</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>14</v>
@@ -4950,7 +4958,7 @@
         <v>16</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>14</v>
@@ -4967,7 +4975,7 @@
         <v>16</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>14</v>
@@ -4984,7 +4992,7 @@
         <v>16</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>14</v>
@@ -5001,7 +5009,7 @@
         <v>16</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>14</v>
@@ -5018,7 +5026,7 @@
         <v>16</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>14</v>
@@ -5035,7 +5043,7 @@
         <v>16</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>14</v>
@@ -5052,7 +5060,7 @@
         <v>16</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>14</v>
@@ -5069,7 +5077,7 @@
         <v>16</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>14</v>
@@ -5085,8 +5093,8 @@
       <c r="B213" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C213" s="3" t="s">
-        <v>179</v>
+      <c r="C213" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>14</v>
@@ -5102,8 +5110,8 @@
       <c r="B214" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C214" s="3" t="s">
-        <v>180</v>
+      <c r="C214" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>14</v>
@@ -5120,7 +5128,7 @@
         <v>16</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>14</v>
@@ -5136,8 +5144,8 @@
       <c r="B216" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C216" s="1" t="s">
-        <v>190</v>
+      <c r="C216" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>14</v>
@@ -5154,7 +5162,7 @@
         <v>16</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>14</v>
@@ -5171,12 +5179,46 @@
         <v>16</v>
       </c>
       <c r="C218" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F218" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A219" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F219" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A220" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C220" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E218" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F218" s="1" t="s">
+      <c r="E220" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F220" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new Indicator FT Factoring
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="237">
   <si>
     <t>Action</t>
   </si>
@@ -811,12 +811,15 @@
   </si>
   <si>
     <t>IND_37_SUPER</t>
+  </si>
+  <si>
+    <t>INDICATOR_IND_XRA_FACTORING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1422,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G220"/>
+  <dimension ref="A1:G221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E218" sqref="E218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -5219,6 +5222,23 @@
         <v>14</v>
       </c>
       <c r="F220" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A221" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F221" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5266,21 +5286,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -5394,17 +5399,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5418,17 +5439,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Create new Variable XRA Factoring
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -813,7 +813,7 @@
     <t>IND_37_SUPER</t>
   </si>
   <si>
-    <t>INDICATOR_IND_XRA_FACTORING</t>
+    <t>INDICATOR_276_XRA_FACTORING</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1428,7 @@
   <dimension ref="A1:G221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E218" sqref="E218"/>
+      <selection activeCell="C221" sqref="C221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -5286,6 +5286,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -5399,22 +5414,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5428,27 +5451,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
aggiornamento excel banche estere e it
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="238">
   <si>
     <t>Action</t>
   </si>
@@ -814,12 +814,15 @@
   </si>
   <si>
     <t>INDICATOR_IND_XRA_FACTORING</t>
+  </si>
+  <si>
+    <t>INDICATOR_88</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1425,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G221"/>
+  <dimension ref="A1:G222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E218" sqref="E218"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -3839,7 +3842,7 @@
         <v>16</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>62</v>
+        <v>237</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>14</v>
@@ -3856,7 +3859,7 @@
         <v>16</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>14</v>
@@ -3873,7 +3876,7 @@
         <v>16</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>14</v>
@@ -3890,7 +3893,7 @@
         <v>16</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>14</v>
@@ -3907,7 +3910,7 @@
         <v>16</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>14</v>
@@ -3924,7 +3927,7 @@
         <v>16</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>14</v>
@@ -3941,7 +3944,7 @@
         <v>16</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>14</v>
@@ -3958,7 +3961,7 @@
         <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>14</v>
@@ -3975,7 +3978,7 @@
         <v>16</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>14</v>
@@ -3992,7 +3995,7 @@
         <v>16</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>14</v>
@@ -4009,7 +4012,7 @@
         <v>16</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>14</v>
@@ -4026,7 +4029,7 @@
         <v>16</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>14</v>
@@ -4043,7 +4046,7 @@
         <v>16</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>14</v>
@@ -4060,7 +4063,7 @@
         <v>16</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>14</v>
@@ -4077,7 +4080,7 @@
         <v>16</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>14</v>
@@ -4094,7 +4097,7 @@
         <v>16</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>14</v>
@@ -4111,7 +4114,7 @@
         <v>16</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>14</v>
@@ -4128,7 +4131,7 @@
         <v>16</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>14</v>
@@ -4145,7 +4148,7 @@
         <v>16</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>14</v>
@@ -4162,7 +4165,7 @@
         <v>16</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>14</v>
@@ -4179,7 +4182,7 @@
         <v>16</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>14</v>
@@ -4196,7 +4199,7 @@
         <v>16</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>14</v>
@@ -4213,7 +4216,7 @@
         <v>16</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>14</v>
@@ -4230,7 +4233,7 @@
         <v>16</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>14</v>
@@ -4247,7 +4250,7 @@
         <v>16</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>14</v>
@@ -4264,7 +4267,7 @@
         <v>16</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>14</v>
@@ -4281,7 +4284,7 @@
         <v>16</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>14</v>
@@ -4298,7 +4301,7 @@
         <v>16</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>14</v>
@@ -4315,7 +4318,7 @@
         <v>16</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>14</v>
@@ -4332,7 +4335,7 @@
         <v>16</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>14</v>
@@ -4349,7 +4352,7 @@
         <v>16</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>14</v>
@@ -4366,7 +4369,7 @@
         <v>16</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>14</v>
@@ -4383,7 +4386,7 @@
         <v>16</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>14</v>
@@ -4400,7 +4403,7 @@
         <v>16</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>14</v>
@@ -4417,7 +4420,7 @@
         <v>16</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>14</v>
@@ -4434,7 +4437,7 @@
         <v>16</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>14</v>
@@ -4451,7 +4454,7 @@
         <v>16</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>14</v>
@@ -4468,7 +4471,7 @@
         <v>16</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>14</v>
@@ -4485,7 +4488,7 @@
         <v>16</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>14</v>
@@ -4502,7 +4505,7 @@
         <v>16</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>14</v>
@@ -4519,7 +4522,7 @@
         <v>16</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>14</v>
@@ -4536,7 +4539,7 @@
         <v>16</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>14</v>
@@ -4553,7 +4556,7 @@
         <v>16</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>14</v>
@@ -4570,7 +4573,7 @@
         <v>16</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>14</v>
@@ -4587,7 +4590,7 @@
         <v>16</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>14</v>
@@ -4604,7 +4607,7 @@
         <v>16</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>14</v>
@@ -4621,7 +4624,7 @@
         <v>16</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>14</v>
@@ -4638,7 +4641,7 @@
         <v>16</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>14</v>
@@ -4655,7 +4658,7 @@
         <v>16</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>14</v>
@@ -4672,7 +4675,7 @@
         <v>16</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>14</v>
@@ -4689,7 +4692,7 @@
         <v>16</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>14</v>
@@ -4706,7 +4709,7 @@
         <v>16</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>14</v>
@@ -4723,7 +4726,7 @@
         <v>16</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>14</v>
@@ -4740,7 +4743,7 @@
         <v>16</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>14</v>
@@ -4757,7 +4760,7 @@
         <v>16</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>14</v>
@@ -4774,7 +4777,7 @@
         <v>16</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>14</v>
@@ -4791,7 +4794,7 @@
         <v>16</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>14</v>
@@ -4808,7 +4811,7 @@
         <v>16</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>14</v>
@@ -4825,7 +4828,7 @@
         <v>16</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>14</v>
@@ -4842,7 +4845,7 @@
         <v>16</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>14</v>
@@ -4859,7 +4862,7 @@
         <v>16</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>14</v>
@@ -4876,7 +4879,7 @@
         <v>16</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>14</v>
@@ -4893,7 +4896,7 @@
         <v>16</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>14</v>
@@ -4910,7 +4913,7 @@
         <v>16</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>14</v>
@@ -4927,7 +4930,7 @@
         <v>16</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>14</v>
@@ -4944,7 +4947,7 @@
         <v>16</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>14</v>
@@ -4961,7 +4964,7 @@
         <v>16</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>14</v>
@@ -4978,7 +4981,7 @@
         <v>16</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>14</v>
@@ -4995,7 +4998,7 @@
         <v>16</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>14</v>
@@ -5012,7 +5015,7 @@
         <v>16</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>14</v>
@@ -5029,7 +5032,7 @@
         <v>16</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>14</v>
@@ -5046,7 +5049,7 @@
         <v>16</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>14</v>
@@ -5063,7 +5066,7 @@
         <v>16</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>14</v>
@@ -5080,7 +5083,7 @@
         <v>16</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>14</v>
@@ -5097,7 +5100,7 @@
         <v>16</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>14</v>
@@ -5114,7 +5117,7 @@
         <v>16</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>14</v>
@@ -5130,8 +5133,8 @@
       <c r="B215" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C215" s="3" t="s">
-        <v>179</v>
+      <c r="C215" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>14</v>
@@ -5148,7 +5151,7 @@
         <v>16</v>
       </c>
       <c r="C216" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>14</v>
@@ -5165,7 +5168,7 @@
         <v>16</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>14</v>
@@ -5181,8 +5184,8 @@
       <c r="B218" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C218" s="1" t="s">
-        <v>190</v>
+      <c r="C218" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="E218" s="1" t="s">
         <v>14</v>
@@ -5198,8 +5201,8 @@
       <c r="B219" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C219" s="3" t="s">
-        <v>182</v>
+      <c r="C219" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="E219" s="1" t="s">
         <v>14</v>
@@ -5215,8 +5218,8 @@
       <c r="B220" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C220" s="1" t="s">
-        <v>191</v>
+      <c r="C220" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>14</v>
@@ -5232,13 +5235,30 @@
       <c r="B221" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C221" s="3" t="s">
+      <c r="C221" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A222" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C222" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="E221" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F221" s="1" t="s">
+      <c r="E222" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F222" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5286,6 +5306,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -5399,22 +5434,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5428,27 +5471,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add new indicator XRA Factoring
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/07_LIB_EWS_IT/07_LibFormula.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tools\progetto Intesa\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dati\DEV\GitRepoAAAP\client-intesa\earlywarning-pom\earlywarning-config\src\baf-configuration\07_LIB_EWS_IT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -813,16 +813,16 @@
     <t>IND_37_SUPER</t>
   </si>
   <si>
-    <t>INDICATOR_IND_XRA_FACTORING</t>
-  </si>
-  <si>
     <t>INDICATOR_88</t>
+  </si>
+  <si>
+    <t>INDICATOR_276_XRA_FACTORING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1430,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C231" sqref="C231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -3842,7 +3842,7 @@
         <v>16</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>14</v>
@@ -5253,7 +5253,7 @@
         <v>16</v>
       </c>
       <c r="C222" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>14</v>
@@ -5306,21 +5306,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -5434,17 +5419,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5458,17 +5459,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3101153D-8A60-4FAA-A016-5BFDF61D07EE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>